<commit_message>
start of the third part
</commit_message>
<xml_diff>
--- a/实验结果03_19.xlsx
+++ b/实验结果03_19.xlsx
@@ -4,15 +4,17 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="结果统计" sheetId="1" r:id="rId1"/>
     <sheet name="需要训练的模型" sheetId="2" r:id="rId2"/>
     <sheet name="数据库统计" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="感受野计算" sheetId="4" r:id="rId4"/>
+    <sheet name="200类目录" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="351">
   <si>
     <t>语言</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -562,6 +564,674 @@
   <si>
     <t>600k</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gpu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coco</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类别数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VOC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ILSVRC DET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">accordion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">airplane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">antelope </t>
+  </si>
+  <si>
+    <t xml:space="preserve">apple </t>
+  </si>
+  <si>
+    <t xml:space="preserve">armadillo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">artichoke </t>
+  </si>
+  <si>
+    <t xml:space="preserve">axe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">baby bed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">backpack </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bagel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">balance beam </t>
+  </si>
+  <si>
+    <t xml:space="preserve">banana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">band aid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">banjo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">baseball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">basketball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bathing cap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">beaker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bell pepper </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bench </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bicycle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">binder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bird </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bookshelf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bow tie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bowl </t>
+  </si>
+  <si>
+    <t xml:space="preserve">brassiere </t>
+  </si>
+  <si>
+    <t xml:space="preserve">burrito </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">butterfly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">camel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">can opener </t>
+  </si>
+  <si>
+    <t xml:space="preserve">car </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cattle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cello </t>
+  </si>
+  <si>
+    <t xml:space="preserve">centipede </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chain saw </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chair </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cocktail shaker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">coffee maker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer keyboard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">computer mouse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">corkscrew </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cream </t>
+  </si>
+  <si>
+    <t xml:space="preserve">croquet ball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">crutch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cucumber </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cup or mug </t>
+  </si>
+  <si>
+    <t xml:space="preserve">diaper </t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital clock </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dishwasher </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dog </t>
+  </si>
+  <si>
+    <t xml:space="preserve">domestic cat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dragonfly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">drum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dumbbell </t>
+  </si>
+  <si>
+    <t xml:space="preserve">electric fan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">elephant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">face powder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fig </t>
+  </si>
+  <si>
+    <t xml:space="preserve">filing cabinet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">flower pot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">flute </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fox </t>
+  </si>
+  <si>
+    <t xml:space="preserve">french horn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">frog </t>
+  </si>
+  <si>
+    <t xml:space="preserve">frying pan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">giant panda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">goldfish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">golf ball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">golfcart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">guacamole </t>
+  </si>
+  <si>
+    <t xml:space="preserve">guitar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hair dryer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hair spray </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hamburger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hammer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hamster </t>
+  </si>
+  <si>
+    <t xml:space="preserve">harmonica </t>
+  </si>
+  <si>
+    <t xml:space="preserve">harp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hat with a wide brim </t>
+  </si>
+  <si>
+    <t xml:space="preserve">head cabbage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">helmet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hippopotamus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">horizontal bar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">horse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hotdog </t>
+  </si>
+  <si>
+    <t xml:space="preserve">iPod </t>
+  </si>
+  <si>
+    <t xml:space="preserve">isopod </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jellyfish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">koala bear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ladle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ladybug </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lamp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">laptop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lemon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lipstick </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lizard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lobster </t>
+  </si>
+  <si>
+    <t xml:space="preserve">maillot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">maraca </t>
+  </si>
+  <si>
+    <t xml:space="preserve">microphone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">microwave </t>
+  </si>
+  <si>
+    <t xml:space="preserve">milk can </t>
+  </si>
+  <si>
+    <t xml:space="preserve">miniskirt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">monkey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">motorcycle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mushroom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">neck brace </t>
+  </si>
+  <si>
+    <t xml:space="preserve">oboe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">orange </t>
+  </si>
+  <si>
+    <t xml:space="preserve">otter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pencil box </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pencil sharpener </t>
+  </si>
+  <si>
+    <t xml:space="preserve">perfume </t>
+  </si>
+  <si>
+    <t xml:space="preserve">person </t>
+  </si>
+  <si>
+    <t xml:space="preserve">piano </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pineapple </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ping-pong ball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pitcher </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pizza </t>
+  </si>
+  <si>
+    <t xml:space="preserve">plastic bag </t>
+  </si>
+  <si>
+    <t xml:space="preserve">plate rack </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pomegranate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">popsicle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">porcupine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">power drill </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pretzel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">printer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">puck </t>
+  </si>
+  <si>
+    <t xml:space="preserve">punching bag </t>
+  </si>
+  <si>
+    <t xml:space="preserve">purse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rabbit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">racket </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ray </t>
+  </si>
+  <si>
+    <t xml:space="preserve">red panda </t>
+  </si>
+  <si>
+    <t xml:space="preserve">refrigerator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">remote control </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rubber eraser </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rugby ball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruler </t>
+  </si>
+  <si>
+    <t xml:space="preserve">salt or pepper shaker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">saxophone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">scorpion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">screwdriver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">seal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheep </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ski </t>
+  </si>
+  <si>
+    <t xml:space="preserve">skunk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">snail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">snake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">snowmobile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">snowplow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">soap dispenser </t>
+  </si>
+  <si>
+    <t xml:space="preserve">soccer ball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sofa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">spatula </t>
+  </si>
+  <si>
+    <t xml:space="preserve">squirrel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">starfish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stethoscope </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stove </t>
+  </si>
+  <si>
+    <t xml:space="preserve">strainer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">strawberry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">stretcher </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sunglasses </t>
+  </si>
+  <si>
+    <t xml:space="preserve">swimming trunks </t>
+  </si>
+  <si>
+    <t xml:space="preserve">swine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">syringe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tape player </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tennis ball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tick </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">toaster </t>
+  </si>
+  <si>
+    <t xml:space="preserve">traffic light </t>
+  </si>
+  <si>
+    <t xml:space="preserve">train </t>
+  </si>
+  <si>
+    <t xml:space="preserve">trombone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">trumpet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">turtle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tv or monitor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">unicycle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacuum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">violin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">volleyball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">waffle iron </t>
+  </si>
+  <si>
+    <t xml:space="preserve">washer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">water bottle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">watercraft </t>
+  </si>
+  <si>
+    <t xml:space="preserve">whale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wine bottle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">zebra </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Class name in 
+PASCAL VOC 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="CMBX8"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(20 classes) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">aeroplane </t>
+  </si>
+  <si>
+    <t xml:space="preserve">boat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bottle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dining table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">motorbike </t>
+  </si>
+  <si>
+    <t xml:space="preserve">potted plant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tv/monitor </t>
   </si>
 </sst>
 </file>
@@ -571,7 +1241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,6 +1264,26 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="CMTI8"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="CMR8"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="CMBX8"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -700,7 +1390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -732,6 +1422,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -740,6 +1433,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1027,7 +1735,7 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="8" max="8" width="15.125" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
@@ -1035,7 +1743,7 @@
     <col min="11" max="11" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="4:11" ht="28.5">
       <c r="D3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1061,17 +1769,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D4" s="21" t="s">
+    <row r="4" spans="4:11">
+      <c r="D4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="20" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1087,11 +1795,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="20"/>
+    <row r="5" spans="4:11">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1105,17 +1813,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D6" s="21" t="s">
+    <row r="6" spans="4:11">
+      <c r="D6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="20" t="s">
         <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -1131,11 +1839,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="20"/>
+    <row r="7" spans="4:11">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1149,17 +1857,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D8" s="21" t="s">
+    <row r="8" spans="4:11">
+      <c r="D8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="20" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1175,11 +1883,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="20"/>
+    <row r="9" spans="4:11">
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1193,7 +1901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="4:11">
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1219,7 +1927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="4:11">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1250,11 +1958,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="16.25" customWidth="1"/>
     <col min="4" max="4" width="15.625" customWidth="1"/>
@@ -1263,12 +1971,12 @@
     <col min="8" max="8" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1318,7 +2026,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15" thickBot="1">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1347,7 +2055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1385,7 +2093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="B5">
         <v>3</v>
       </c>
@@ -1423,7 +2131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="B6">
         <v>1</v>
       </c>
@@ -1461,7 +2169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="15" thickBot="1">
       <c r="B7">
         <v>4</v>
       </c>
@@ -1499,7 +2207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="15" thickBot="1">
       <c r="B8">
         <v>9</v>
       </c>
@@ -1528,7 +2236,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="15" thickBot="1">
       <c r="B9">
         <v>8</v>
       </c>
@@ -1566,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15" thickBot="1">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1604,7 +2312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="B11">
         <v>5</v>
       </c>
@@ -1642,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="15" thickBot="1">
       <c r="B12">
         <v>6</v>
       </c>
@@ -1680,7 +2388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="B13">
         <v>11</v>
       </c>
@@ -1702,9 +2410,11 @@
       <c r="N13" t="s">
         <v>119</v>
       </c>
-      <c r="P13" s="17"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P13" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="B14">
         <v>13</v>
       </c>
@@ -1726,9 +2436,11 @@
       <c r="N14" t="s">
         <v>121</v>
       </c>
-      <c r="P14" s="17"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P14" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="B15">
         <v>10</v>
       </c>
@@ -1747,8 +2459,11 @@
       <c r="G15" s="15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P15" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" thickBot="1">
       <c r="B16">
         <v>12</v>
       </c>
@@ -1770,8 +2485,11 @@
       <c r="N16" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" thickBot="1">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1794,11 +2512,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="B19">
         <v>15</v>
       </c>
@@ -1824,10 +2542,10 @@
         <v>6</v>
       </c>
       <c r="N19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="B20">
         <v>16</v>
       </c>
@@ -1846,12 +2564,15 @@
       <c r="G20" s="16" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="E21" s="8"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="B22">
         <v>17</v>
       </c>
@@ -1886,7 +2607,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="B23">
         <v>18</v>
       </c>
@@ -1921,7 +2642,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>125</v>
       </c>
@@ -1935,7 +2656,7 @@
         <v>42</v>
       </c>
       <c r="E24" s="8">
-        <v>512</v>
+        <v>300</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>46</v>
@@ -1959,7 +2680,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -1997,7 +2718,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -2026,7 +2747,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="C28" t="s">
         <v>60</v>
       </c>
@@ -2052,7 +2773,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2078,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14">
       <c r="C32" t="s">
         <v>64</v>
       </c>
@@ -2104,20 +2825,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M9"/>
+  <dimension ref="B1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13">
       <c r="C1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13">
       <c r="B2" t="s">
         <v>76</v>
       </c>
@@ -2149,7 +2870,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13">
       <c r="B3" t="s">
         <v>77</v>
       </c>
@@ -2176,7 +2897,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13">
       <c r="I4">
         <v>229</v>
       </c>
@@ -2194,7 +2915,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13">
       <c r="I5">
         <v>229</v>
       </c>
@@ -2212,7 +2933,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13">
       <c r="I6">
         <v>3579</v>
       </c>
@@ -2230,7 +2951,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13">
       <c r="I7">
         <v>3579</v>
       </c>
@@ -2248,7 +2969,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13">
       <c r="I8">
         <v>3579</v>
       </c>
@@ -2266,7 +2987,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13">
       <c r="I9">
         <v>3579</v>
       </c>
@@ -2282,6 +3003,35 @@
       </c>
       <c r="M9" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6">
+      <c r="F18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6">
+      <c r="E19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6">
+      <c r="E20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6">
+      <c r="E21" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2299,14 +3049,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="8.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="4:6">
       <c r="D2" t="s">
         <v>91</v>
       </c>
@@ -2317,7 +3067,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="4:6">
       <c r="D3" t="s">
         <v>92</v>
       </c>
@@ -2328,7 +3078,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="4:6">
       <c r="D4" t="s">
         <v>97</v>
       </c>
@@ -2343,4 +3093,770 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:R35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="7.375" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:17">
+      <c r="Q1" s="17"/>
+    </row>
+    <row r="2" spans="3:17">
+      <c r="C2" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q2" s="25"/>
+    </row>
+    <row r="3" spans="3:17" ht="28.5">
+      <c r="C3" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q3" s="25"/>
+    </row>
+    <row r="4" spans="3:17" ht="28.5">
+      <c r="C4" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q4" s="25"/>
+    </row>
+    <row r="5" spans="3:17" ht="28.5">
+      <c r="C5" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q5" s="25"/>
+    </row>
+    <row r="6" spans="3:17" ht="28.5">
+      <c r="C6" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q6" s="25"/>
+    </row>
+    <row r="7" spans="3:17" ht="28.5">
+      <c r="C7" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q7" s="26"/>
+    </row>
+    <row r="8" spans="3:17" ht="28.5">
+      <c r="C8" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q8" s="26"/>
+    </row>
+    <row r="9" spans="3:17" ht="28.5">
+      <c r="C9" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q9" s="25"/>
+    </row>
+    <row r="10" spans="3:17" ht="28.5">
+      <c r="C10" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="L10" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" spans="3:17" ht="42.75">
+      <c r="C11" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" spans="3:17" ht="28.5">
+      <c r="C12" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="3:17" ht="28.5">
+      <c r="C13" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q13" s="26"/>
+    </row>
+    <row r="14" spans="3:17" ht="28.5">
+      <c r="C14" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q14" s="26"/>
+    </row>
+    <row r="15" spans="3:17" ht="28.5">
+      <c r="C15" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q15" s="25"/>
+    </row>
+    <row r="16" spans="3:17" ht="28.5">
+      <c r="C16" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q16" s="25"/>
+    </row>
+    <row r="17" spans="3:18" ht="28.5">
+      <c r="C17" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q17" s="25"/>
+    </row>
+    <row r="18" spans="3:18" ht="28.5">
+      <c r="C18" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q18" s="25"/>
+    </row>
+    <row r="19" spans="3:18" ht="28.5">
+      <c r="C19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q19" s="26"/>
+    </row>
+    <row r="20" spans="3:18" ht="28.5">
+      <c r="C20" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q20" s="25"/>
+    </row>
+    <row r="21" spans="3:18" ht="28.5">
+      <c r="C21" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q21" s="25"/>
+    </row>
+    <row r="22" spans="3:18">
+      <c r="Q22" s="25"/>
+    </row>
+    <row r="23" spans="3:18" ht="14.25" customHeight="1">
+      <c r="M23" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="N23" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="O23" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="P23" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q23" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="R23" s="27" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18">
+      <c r="M24" s="24"/>
+      <c r="N24" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="O24" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="P24" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q24" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="R24" s="27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18">
+      <c r="M25" s="24"/>
+      <c r="N25" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="O25" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="P25" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q25" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="R25" s="23" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18">
+      <c r="M26" s="24"/>
+      <c r="N26" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="O26" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="P26" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q26" s="23" t="s">
+        <v>325</v>
+      </c>
+      <c r="R26" s="23" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18" ht="14.25" customHeight="1"/>
+    <row r="35" ht="27.75" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M23:M26"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
don't know how to write the third part
</commit_message>
<xml_diff>
--- a/实验结果03_19.xlsx
+++ b/实验结果03_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="结果统计" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,6 @@
     <sheet name="200类目录" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="359">
   <si>
     <t>语言</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -275,10 +274,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>字符串</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -312,10 +307,6 @@
   </si>
   <si>
     <t>my</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gpu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1232,6 +1223,46 @@
   </si>
   <si>
     <t xml:space="preserve">tv/monitor </t>
+  </si>
+  <si>
+    <t>ICDAR13-train</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>150k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周五晚上开始跑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my，16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03.29-10.00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no step</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20k, 30k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1425,6 +1456,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1435,18 +1478,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1770,16 +1801,16 @@
       </c>
     </row>
     <row r="4" spans="4:11">
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="24" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1796,10 +1827,10 @@
       </c>
     </row>
     <row r="5" spans="4:11">
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="21"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1814,16 +1845,16 @@
       </c>
     </row>
     <row r="6" spans="4:11">
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="24" t="s">
         <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -1840,10 +1871,10 @@
       </c>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1858,16 +1889,16 @@
       </c>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="24" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1884,10 +1915,10 @@
       </c>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="21"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1956,10 +1987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1973,7 +2004,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1981,7 +2012,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
@@ -2008,22 +2039,22 @@
         <v>38</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>356</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" t="s">
         <v>69</v>
       </c>
-      <c r="N2" t="s">
-        <v>70</v>
-      </c>
       <c r="O2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1">
@@ -2040,7 +2071,7 @@
         <v>300</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -2069,7 +2100,7 @@
         <v>300</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>44</v>
@@ -2084,10 +2115,10 @@
         <v>2</v>
       </c>
       <c r="N4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P4" s="9">
         <v>2</v>
@@ -2107,7 +2138,7 @@
         <v>300</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>45</v>
@@ -2122,10 +2153,10 @@
         <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P5" s="10">
         <v>1</v>
@@ -2145,7 +2176,7 @@
         <v>300</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>50</v>
@@ -2160,10 +2191,10 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="P6" s="10">
         <v>3</v>
@@ -2183,10 +2214,10 @@
         <v>300</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H7" s="8">
         <v>1</v>
@@ -2198,10 +2229,10 @@
         <v>4</v>
       </c>
       <c r="N7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P7" s="11">
         <v>4</v>
@@ -2221,10 +2252,10 @@
         <v>300</v>
       </c>
       <c r="F8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H8" s="8">
         <v>1</v>
@@ -2233,7 +2264,7 @@
         <v>300</v>
       </c>
       <c r="N8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" thickBot="1">
@@ -2262,13 +2293,13 @@
         <v>300</v>
       </c>
       <c r="N9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Q9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R9" s="9">
         <v>1</v>
@@ -2288,25 +2319,25 @@
         <v>300</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="P10" s="9">
         <v>2</v>
       </c>
       <c r="Q10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R10" s="11">
         <v>2</v>
@@ -2329,7 +2360,7 @@
         <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2341,10 +2372,10 @@
         <v>4</v>
       </c>
       <c r="N11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P11" s="10">
         <v>1</v>
@@ -2364,10 +2395,10 @@
         <v>300</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2379,10 +2410,10 @@
         <v>5</v>
       </c>
       <c r="N12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P12" s="11">
         <v>3</v>
@@ -2408,7 +2439,7 @@
         <v>5</v>
       </c>
       <c r="N13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="P13" s="14">
         <v>2</v>
@@ -2434,7 +2465,7 @@
         <v>6</v>
       </c>
       <c r="N14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="P14" s="15">
         <v>4</v>
@@ -2483,13 +2514,13 @@
         <v>3</v>
       </c>
       <c r="N16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="P16" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" thickBot="1">
+    <row r="17" spans="1:15" ht="15" thickBot="1">
       <c r="B17">
         <v>14</v>
       </c>
@@ -2509,16 +2540,16 @@
         <v>7</v>
       </c>
       <c r="N17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="B19">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
@@ -2526,28 +2557,22 @@
       <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="7">
-        <v>512</v>
-      </c>
-      <c r="F19" s="17" t="s">
+      <c r="E19">
+        <v>300</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>46</v>
       </c>
       <c r="G19">
         <v>4</v>
       </c>
-      <c r="I19">
-        <v>500</v>
-      </c>
-      <c r="L19">
-        <v>6</v>
-      </c>
-      <c r="N19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="K19" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="B20">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
@@ -2555,64 +2580,57 @@
       <c r="D20" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="7">
-        <v>512</v>
-      </c>
-      <c r="F20" s="17" t="s">
+      <c r="E20">
+        <v>300</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="N20" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="E21" s="8"/>
-      <c r="F21" s="17"/>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="B22">
-        <v>17</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="7">
-        <v>300</v>
+        <v>512</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G22" t="s">
-        <v>124</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
+      <c r="G22">
+        <v>4</v>
       </c>
       <c r="I22">
         <v>500</v>
       </c>
       <c r="L22">
-        <v>7</v>
-      </c>
-      <c r="M22" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="N22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="B23">
-        <v>18</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>49</v>
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>349</v>
       </c>
       <c r="D23" t="s">
         <v>42</v>
@@ -2623,196 +2641,264 @@
       <c r="F23" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G23" t="s">
-        <v>124</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>500</v>
-      </c>
-      <c r="L23">
-        <v>8</v>
-      </c>
-      <c r="M23" t="s">
-        <v>68</v>
+      <c r="G23" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="N23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24">
-        <v>19</v>
-      </c>
-      <c r="C24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="8">
-        <v>300</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <v>500</v>
-      </c>
-      <c r="J24" t="s">
-        <v>52</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="N24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" t="s">
-        <v>126</v>
-      </c>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="E24" s="8"/>
+      <c r="F24" s="17"/>
+    </row>
+    <row r="25" spans="1:15">
       <c r="B25">
-        <v>20</v>
-      </c>
-      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>49</v>
       </c>
       <c r="D25" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="8">
-        <v>512</v>
-      </c>
-      <c r="F25" s="8" t="s">
+      <c r="E25" s="7">
+        <v>300</v>
+      </c>
+      <c r="F25" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>47</v>
+      <c r="G25" t="s">
+        <v>122</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25">
+        <v>500</v>
+      </c>
+      <c r="L25">
+        <v>7</v>
+      </c>
+      <c r="M25" t="s">
+        <v>67</v>
+      </c>
+      <c r="N25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="7">
+        <v>512</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>500</v>
+      </c>
+      <c r="L26">
+        <v>8</v>
+      </c>
+      <c r="M26" t="s">
+        <v>67</v>
+      </c>
+      <c r="N26" t="s">
+        <v>99</v>
+      </c>
+      <c r="O26" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="8">
         <v>300</v>
       </c>
-      <c r="J25" t="s">
-        <v>52</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="N25" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27">
-        <v>512</v>
-      </c>
-      <c r="F27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" t="s">
-        <v>58</v>
+      <c r="F27" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27" t="s">
-        <v>59</v>
+      <c r="I27">
+        <v>500</v>
+      </c>
+      <c r="J27" t="s">
+        <v>52</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28">
+        <v>42</v>
+      </c>
+      <c r="E28" s="8">
         <v>512</v>
       </c>
-      <c r="F28" t="s">
-        <v>48</v>
-      </c>
-      <c r="G28" t="s">
-        <v>58</v>
+      <c r="F28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28">
+        <v>300</v>
+      </c>
+      <c r="J28" t="s">
+        <v>52</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="N28" t="s">
+        <v>125</v>
+      </c>
+      <c r="O28" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30">
+        <v>512</v>
+      </c>
+      <c r="F30" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
         <v>59</v>
       </c>
-      <c r="N28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
+      <c r="N30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="C31" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E31">
-        <v>300</v>
+        <v>512</v>
       </c>
       <c r="F31" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="G31" t="s">
+        <v>58</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>66</v>
-      </c>
-      <c r="K31">
+        <v>59</v>
+      </c>
+      <c r="N31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34">
+        <v>300</v>
+      </c>
+      <c r="F34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="C32" t="s">
+      <c r="I34" t="s">
+        <v>65</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" t="s">
         <v>64</v>
       </c>
-      <c r="D32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32">
+      <c r="E35">
         <v>512</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F35" t="s">
         <v>46</v>
       </c>
-      <c r="H32">
+      <c r="H35">
         <v>1</v>
       </c>
     </row>
@@ -2825,54 +2911,57 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M21"/>
+  <dimension ref="B1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I5" sqref="I5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="2:13">
+    <row r="1" spans="2:14">
       <c r="C1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14">
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="2:13">
-      <c r="B2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>83</v>
       </c>
-      <c r="J2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L2" t="s">
-        <v>84</v>
-      </c>
-      <c r="M2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13">
+      <c r="N2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3">
         <v>229</v>
@@ -2894,10 +2983,10 @@
         <v>10018.75</v>
       </c>
       <c r="M3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="I4">
         <v>229</v>
       </c>
@@ -2912,10 +3001,10 @@
         <v>20037.5</v>
       </c>
       <c r="M4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14">
       <c r="I5">
         <v>229</v>
       </c>
@@ -2930,10 +3019,13 @@
         <v>40075</v>
       </c>
       <c r="M5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13">
+        <v>128</v>
+      </c>
+      <c r="N5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
       <c r="I6">
         <v>3579</v>
       </c>
@@ -2948,10 +3040,13 @@
         <v>313162.5</v>
       </c>
       <c r="M6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13">
+        <v>129</v>
+      </c>
+      <c r="N6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="I7">
         <v>3579</v>
       </c>
@@ -2966,10 +3061,10 @@
         <v>156581.25</v>
       </c>
       <c r="M7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
       <c r="I8">
         <v>3579</v>
       </c>
@@ -2984,10 +3079,10 @@
         <v>78290.625</v>
       </c>
       <c r="M8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
       <c r="I9">
         <v>3579</v>
       </c>
@@ -3002,17 +3097,20 @@
         <v>626325</v>
       </c>
       <c r="M9" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+      <c r="N9" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="5:6">
       <c r="F18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="5:6">
       <c r="E19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F19">
         <v>80</v>
@@ -3020,7 +3118,7 @@
     </row>
     <row r="20" spans="5:6">
       <c r="E20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F20">
         <v>20</v>
@@ -3028,7 +3126,7 @@
     </row>
     <row r="21" spans="5:6">
       <c r="E21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F21">
         <v>200</v>
@@ -3058,35 +3156,35 @@
   <sheetData>
     <row r="2" spans="4:6">
       <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
         <v>91</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>93</v>
-      </c>
-      <c r="F2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="4:6">
       <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
         <v>92</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>94</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="4:6">
       <c r="D4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
         <v>97</v>
       </c>
-      <c r="E4" t="s">
-        <v>99</v>
-      </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3099,7 +3197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -3115,739 +3213,739 @@
     </row>
     <row r="2" spans="3:17">
       <c r="C2" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>321</v>
-      </c>
-      <c r="Q2" s="25"/>
+        <v>319</v>
+      </c>
+      <c r="Q2" s="21"/>
     </row>
     <row r="3" spans="3:17" ht="28.5">
       <c r="C3" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="Q3" s="25"/>
+        <v>320</v>
+      </c>
+      <c r="Q3" s="21"/>
     </row>
     <row r="4" spans="3:17" ht="28.5">
       <c r="C4" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>323</v>
-      </c>
-      <c r="Q4" s="25"/>
+        <v>321</v>
+      </c>
+      <c r="Q4" s="21"/>
     </row>
     <row r="5" spans="3:17" ht="28.5">
       <c r="C5" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>324</v>
-      </c>
-      <c r="Q5" s="25"/>
+        <v>322</v>
+      </c>
+      <c r="Q5" s="21"/>
     </row>
     <row r="6" spans="3:17" ht="28.5">
       <c r="C6" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q6" s="25"/>
+        <v>323</v>
+      </c>
+      <c r="Q6" s="21"/>
     </row>
     <row r="7" spans="3:17" ht="28.5">
       <c r="C7" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q7" s="26"/>
+        <v>324</v>
+      </c>
+      <c r="Q7" s="22"/>
     </row>
     <row r="8" spans="3:17" ht="28.5">
       <c r="C8" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I8" s="19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q8" s="26"/>
+        <v>325</v>
+      </c>
+      <c r="Q8" s="22"/>
     </row>
     <row r="9" spans="3:17" ht="28.5">
       <c r="C9" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="Q9" s="25"/>
+        <v>326</v>
+      </c>
+      <c r="Q9" s="21"/>
     </row>
     <row r="10" spans="3:17" ht="28.5">
       <c r="C10" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q10" s="25"/>
+        <v>327</v>
+      </c>
+      <c r="Q10" s="21"/>
     </row>
     <row r="11" spans="3:17" ht="42.75">
       <c r="C11" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q11" s="25"/>
+        <v>328</v>
+      </c>
+      <c r="Q11" s="21"/>
     </row>
     <row r="12" spans="3:17" ht="28.5">
       <c r="C12" s="19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q12" s="25"/>
+        <v>329</v>
+      </c>
+      <c r="Q12" s="21"/>
     </row>
     <row r="13" spans="3:17" ht="28.5">
       <c r="C13" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q13" s="26"/>
+        <v>330</v>
+      </c>
+      <c r="Q13" s="22"/>
     </row>
     <row r="14" spans="3:17" ht="28.5">
       <c r="C14" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q14" s="26"/>
+        <v>331</v>
+      </c>
+      <c r="Q14" s="22"/>
     </row>
     <row r="15" spans="3:17" ht="28.5">
       <c r="C15" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q15" s="25"/>
+        <v>332</v>
+      </c>
+      <c r="Q15" s="21"/>
     </row>
     <row r="16" spans="3:17" ht="28.5">
       <c r="C16" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L16" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q16" s="25"/>
+        <v>333</v>
+      </c>
+      <c r="Q16" s="21"/>
     </row>
     <row r="17" spans="3:18" ht="28.5">
       <c r="C17" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q17" s="25"/>
+        <v>334</v>
+      </c>
+      <c r="Q17" s="21"/>
     </row>
     <row r="18" spans="3:18" ht="28.5">
       <c r="C18" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q18" s="25"/>
+        <v>335</v>
+      </c>
+      <c r="Q18" s="21"/>
     </row>
     <row r="19" spans="3:18" ht="28.5">
       <c r="C19" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q19" s="26"/>
+        <v>336</v>
+      </c>
+      <c r="Q19" s="22"/>
     </row>
     <row r="20" spans="3:18" ht="28.5">
       <c r="C20" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>339</v>
-      </c>
-      <c r="Q20" s="25"/>
+        <v>337</v>
+      </c>
+      <c r="Q20" s="21"/>
     </row>
     <row r="21" spans="3:18" ht="28.5">
       <c r="C21" s="19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L21" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q21" s="21"/>
+    </row>
+    <row r="22" spans="3:18">
+      <c r="Q22" s="21"/>
+    </row>
+    <row r="23" spans="3:18" ht="14.25" customHeight="1">
+      <c r="M23" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="N23" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="Q21" s="25"/>
-    </row>
-    <row r="22" spans="3:18">
-      <c r="Q22" s="25"/>
-    </row>
-    <row r="23" spans="3:18" ht="14.25" customHeight="1">
-      <c r="M23" s="24" t="s">
+      <c r="O23" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="P23" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q23" s="23" t="s">
         <v>341</v>
       </c>
-      <c r="N23" s="23" t="s">
+      <c r="R23" s="23" t="s">
         <v>342</v>
       </c>
-      <c r="O23" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="P23" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q23" s="27" t="s">
+    </row>
+    <row r="24" spans="3:18">
+      <c r="M24" s="27"/>
+      <c r="N24" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="O24" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="P24" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="R23" s="27" t="s">
+      <c r="Q24" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="R24" s="23" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="3:18">
-      <c r="M24" s="24"/>
-      <c r="N24" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="O24" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="P24" s="23" t="s">
+    <row r="25" spans="3:18">
+      <c r="M25" s="27"/>
+      <c r="N25" s="23" t="s">
         <v>345</v>
       </c>
-      <c r="Q24" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="R24" s="27" t="s">
+      <c r="O25" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="P25" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q25" s="20" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="25" spans="3:18">
-      <c r="M25" s="24"/>
-      <c r="N25" s="27" t="s">
+      <c r="R25" s="20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18">
+      <c r="M26" s="27"/>
+      <c r="N26" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="O25" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="P25" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q25" s="23" t="s">
+      <c r="O26" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="P26" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q26" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="R26" s="20" t="s">
         <v>348</v>
-      </c>
-      <c r="R25" s="23" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="26" spans="3:18">
-      <c r="M26" s="24"/>
-      <c r="N26" s="27" t="s">
-        <v>349</v>
-      </c>
-      <c r="O26" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="P26" s="23" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q26" s="23" t="s">
-        <v>325</v>
-      </c>
-      <c r="R26" s="23" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="29" spans="3:18" ht="14.25" customHeight="1"/>
@@ -3858,5 +3956,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add table to third part
</commit_message>
<xml_diff>
--- a/实验结果03_19.xlsx
+++ b/实验结果03_19.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="434">
   <si>
     <t>语言</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1421,10 +1421,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>my1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>180k</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1546,10 +1542,6 @@
   </si>
   <si>
     <t>30k</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3632,8 +3624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20:Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4804,7 +4796,7 @@
       </c>
       <c r="I18" s="41"/>
       <c r="J18" s="45" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="K18" s="60"/>
       <c r="L18" s="60"/>
@@ -4908,7 +4900,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C20" s="42">
         <v>512</v>
@@ -5003,23 +4995,31 @@
         <v>391</v>
       </c>
       <c r="I21" s="45"/>
-      <c r="J21" s="45" t="s">
-        <v>402</v>
-      </c>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60" t="e">
+      <c r="J21" s="45">
+        <v>300</v>
+      </c>
+      <c r="K21" s="60">
+        <v>73.424999999999997</v>
+      </c>
+      <c r="L21" s="60">
+        <v>82.546000000000006</v>
+      </c>
+      <c r="M21" s="60">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>77.718807342390576</v>
       </c>
       <c r="N21" s="45">
         <v>512</v>
       </c>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="60" t="e">
+      <c r="O21" s="60">
+        <v>76.072999999999993</v>
+      </c>
+      <c r="P21" s="60">
+        <v>51.579000000000001</v>
+      </c>
+      <c r="Q21" s="60">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>61.476032760943824</v>
       </c>
       <c r="R21" s="45">
         <v>700</v>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="I22" s="45"/>
       <c r="J22" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K22" s="60"/>
       <c r="L22" s="60"/>
@@ -5334,21 +5334,31 @@
         <v>368</v>
       </c>
       <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60" t="e">
+      <c r="J26" s="6">
+        <v>300</v>
+      </c>
+      <c r="K26" s="60">
+        <v>58.904000000000003</v>
+      </c>
+      <c r="L26" s="60">
+        <v>75.703999999999994</v>
+      </c>
+      <c r="M26" s="60">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>66.255622489005106</v>
       </c>
       <c r="N26" s="45">
         <v>512</v>
       </c>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="60" t="e">
+      <c r="O26" s="60">
+        <v>66.849000000000004</v>
+      </c>
+      <c r="P26" s="60">
+        <v>57.457000000000001</v>
+      </c>
+      <c r="Q26" s="60">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>61.798191446913265</v>
       </c>
       <c r="R26" s="45">
         <v>700</v>
@@ -5374,7 +5384,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C27" s="6">
         <v>512</v>
@@ -5389,16 +5399,16 @@
         <v>8</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>401</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J27" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K27" s="60">
         <v>71.688999999999993</v>
@@ -5411,7 +5421,7 @@
         <v>74.619593414900081</v>
       </c>
       <c r="N27" s="45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O27" s="60">
         <v>82.009</v>
@@ -5420,11 +5430,11 @@
         <v>76.686999999999998</v>
       </c>
       <c r="Q27" s="60">
-        <f t="shared" ref="Q27" si="9">2/(1/O27+1/P27)</f>
+        <f t="shared" ref="Q27:Q28" si="9">2/(1/O27+1/P27)</f>
         <v>79.258761191208336</v>
       </c>
       <c r="R27" s="45" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="S27" s="60">
         <v>70.411000000000001</v>
@@ -5437,7 +5447,7 @@
         <v>75.551199523408286</v>
       </c>
       <c r="V27" s="45" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="W27" s="60">
         <v>79.543000000000006</v>
@@ -5470,16 +5480,16 @@
         <v>8</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J28" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K28" s="60">
         <v>69.772000000000006</v>
@@ -5492,7 +5502,7 @@
         <v>74.536762545736181</v>
       </c>
       <c r="N28" s="45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O28" s="60">
         <v>82.1</v>
@@ -5500,11 +5510,12 @@
       <c r="P28" s="60">
         <v>82.856999999999999</v>
       </c>
-      <c r="Q28" s="60" t="s">
-        <v>434</v>
+      <c r="Q28" s="60">
+        <f t="shared" si="9"/>
+        <v>82.476763035215228</v>
       </c>
       <c r="R28" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="S28" s="60">
         <v>70.775999999999996</v>
@@ -5517,7 +5528,7 @@
         <v>75.279033459019644</v>
       </c>
       <c r="V28" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="W28" s="60">
         <v>81.37</v>
@@ -5547,8 +5558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:S27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25:R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5810,10 +5821,10 @@
         <v>4</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="K12" s="30">
         <v>10</v>
@@ -6320,10 +6331,10 @@
         <v>4</v>
       </c>
       <c r="Q25" t="s">
+        <v>427</v>
+      </c>
+      <c r="R25" t="s">
         <v>428</v>
-      </c>
-      <c r="R25" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6370,10 +6381,10 @@
         <v>4</v>
       </c>
       <c r="Q26" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="R26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="27" spans="2:18">
@@ -6396,10 +6407,10 @@
         <v>4</v>
       </c>
       <c r="Q27" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="R27" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -6550,7 +6561,7 @@
         <v>129</v>
       </c>
       <c r="N6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="2:14">
@@ -6607,7 +6618,7 @@
         <v>132</v>
       </c>
       <c r="N9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="5:6">
@@ -6747,7 +6758,7 @@
     </row>
     <row r="2" spans="2:16" ht="15.75">
       <c r="B2" s="69" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
@@ -7422,7 +7433,7 @@
     </row>
     <row r="23" spans="2:17" ht="15" thickBot="1">
       <c r="M23" s="70" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="N23" s="71"/>
       <c r="O23" s="71"/>
@@ -7450,7 +7461,7 @@
     <row r="25" spans="2:17">
       <c r="L25" s="67"/>
       <c r="M25" s="46" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N25" s="43" t="s">
         <v>175</v>
@@ -7520,7 +7531,7 @@
     </row>
     <row r="32" spans="2:17">
       <c r="L32" s="43" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="M32" s="43" t="s">
         <v>175</v>
@@ -7571,26 +7582,26 @@
     </row>
     <row r="35" spans="12:19">
       <c r="R35" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="S35" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="36" spans="12:19" ht="228">
       <c r="R36" s="58" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="S36" s="59" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="37" spans="12:19" ht="229.5">
       <c r="R37" s="58" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="S37" s="57" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish experiments in third part
</commit_message>
<xml_diff>
--- a/实验结果03_19.xlsx
+++ b/实验结果03_19.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7560" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="结果统计" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="433">
   <si>
     <t>语言</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1509,10 +1509,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>jianyun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cocoICDAR13SCUT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1545,7 +1541,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>xiaodong</t>
+    <t xml:space="preserve">  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2004,7 +2000,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2154,6 +2150,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2507,16 +2506,16 @@
       </c>
     </row>
     <row r="4" spans="4:11">
-      <c r="D4" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="65" t="s">
+      <c r="D4" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="65" t="s">
+      <c r="F4" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="63" t="s">
+      <c r="G4" s="64" t="s">
         <v>33</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -2533,10 +2532,10 @@
       </c>
     </row>
     <row r="5" spans="4:11">
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="64"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2551,16 +2550,16 @@
       </c>
     </row>
     <row r="6" spans="4:11">
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F6" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="63" t="s">
+      <c r="G6" s="64" t="s">
         <v>32</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -2577,10 +2576,10 @@
       </c>
     </row>
     <row r="7" spans="4:11">
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="64"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="65"/>
       <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
@@ -2595,16 +2594,16 @@
       </c>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="65" t="s">
+      <c r="F8" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="63" t="s">
+      <c r="G8" s="64" t="s">
         <v>33</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -2621,10 +2620,10 @@
       </c>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="64"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="65"/>
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
@@ -3624,8 +3623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20:Q20"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3651,29 +3650,29 @@
       <c r="H1" s="45"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
-      <c r="K1" s="65" t="s">
+      <c r="K1" s="66" t="s">
         <v>396</v>
       </c>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
       <c r="N1" s="45"/>
-      <c r="O1" s="65" t="s">
+      <c r="O1" s="66" t="s">
         <v>396</v>
       </c>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
       <c r="R1" s="45"/>
-      <c r="S1" s="65" t="s">
+      <c r="S1" s="66" t="s">
         <v>396</v>
       </c>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
       <c r="V1" s="45"/>
-      <c r="W1" s="65" t="s">
+      <c r="W1" s="66" t="s">
         <v>396</v>
       </c>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="45" t="s">
@@ -4394,7 +4393,7 @@
       <c r="L12" s="60">
         <v>79.606999999999999</v>
       </c>
-      <c r="M12" s="60">
+      <c r="M12" s="61">
         <f t="shared" si="0"/>
         <v>72.564637174070583</v>
       </c>
@@ -4746,7 +4745,7 @@
       <c r="P17" s="60">
         <v>81.236999999999995</v>
       </c>
-      <c r="Q17" s="60">
+      <c r="Q17" s="61">
         <f t="shared" si="6"/>
         <v>76.982249747389687</v>
       </c>
@@ -4795,23 +4794,30 @@
         <v>368</v>
       </c>
       <c r="I18" s="41"/>
-      <c r="J18" s="45" t="s">
-        <v>433</v>
-      </c>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60" t="e">
+      <c r="J18" s="63">
+        <v>300</v>
+      </c>
+      <c r="K18" s="60">
+        <v>62.74</v>
+      </c>
+      <c r="L18" s="60">
+        <v>76.846000000000004</v>
+      </c>
+      <c r="M18" s="60">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>69.080252174286812</v>
       </c>
       <c r="N18" s="45">
         <v>512</v>
       </c>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+      <c r="O18" s="60">
+        <v>73.606999999999999</v>
+      </c>
+      <c r="P18" s="60">
+        <v>79.331000000000003</v>
+      </c>
+      <c r="Q18" s="61" t="s">
+        <v>432</v>
       </c>
       <c r="R18" s="45">
         <v>700</v>
@@ -4858,23 +4864,31 @@
         <v>391</v>
       </c>
       <c r="I19" s="45"/>
-      <c r="J19" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60" t="e">
+      <c r="J19" s="63">
+        <v>300</v>
+      </c>
+      <c r="K19" s="60">
+        <v>74.703000000000003</v>
+      </c>
+      <c r="L19" s="60">
+        <v>83.983999999999995</v>
+      </c>
+      <c r="M19" s="61">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>79.072094777770076</v>
       </c>
       <c r="N19" s="45">
         <v>512</v>
       </c>
-      <c r="O19" s="60"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="60" t="e">
+      <c r="O19" s="60">
+        <v>74.247</v>
+      </c>
+      <c r="P19" s="60">
+        <v>59.779000000000003</v>
+      </c>
+      <c r="Q19" s="60">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>66.232095459090033</v>
       </c>
       <c r="R19" s="45">
         <v>700</v>
@@ -4900,7 +4914,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C20" s="42">
         <v>512</v>
@@ -5066,23 +5080,31 @@
         <v>391</v>
       </c>
       <c r="I22" s="45"/>
-      <c r="J22" s="45" t="s">
-        <v>424</v>
-      </c>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60" t="e">
+      <c r="J22" s="45">
+        <v>300</v>
+      </c>
+      <c r="K22" s="60">
+        <v>70.046000000000006</v>
+      </c>
+      <c r="L22" s="60">
+        <v>82.296000000000006</v>
+      </c>
+      <c r="M22" s="60">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>75.678481521839018</v>
       </c>
       <c r="N22" s="45">
         <v>512</v>
       </c>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="60" t="e">
+      <c r="O22" s="60">
+        <v>80.912999999999997</v>
+      </c>
+      <c r="P22" s="60">
+        <v>83.584999999999994</v>
+      </c>
+      <c r="Q22" s="61">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <v>82.227298872934625</v>
       </c>
       <c r="R22" s="45">
         <v>700</v>
@@ -5384,7 +5406,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C27" s="6">
         <v>512</v>
@@ -5582,26 +5604,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:19">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="67" t="s">
         <v>379</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="K3" s="66" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="K3" s="67" t="s">
         <v>381</v>
       </c>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="29">
@@ -5780,26 +5802,26 @@
       </c>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="67" t="s">
         <v>380</v>
       </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="L11" s="66" t="s">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="L11" s="67" t="s">
         <v>382</v>
       </c>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="66"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="67"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="2">
@@ -5821,10 +5843,10 @@
         <v>4</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>431</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>432</v>
       </c>
       <c r="K12" s="30">
         <v>10</v>
@@ -6124,16 +6146,16 @@
       <c r="I20" s="39" t="s">
         <v>368</v>
       </c>
-      <c r="K20" s="66" t="s">
+      <c r="K20" s="67" t="s">
         <v>384</v>
       </c>
-      <c r="L20" s="66"/>
-      <c r="M20" s="66"/>
-      <c r="N20" s="66"/>
-      <c r="O20" s="66"/>
-      <c r="P20" s="66"/>
-      <c r="Q20" s="66"/>
-      <c r="R20" s="66"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
     </row>
     <row r="21" spans="2:18">
       <c r="K21" s="29">
@@ -6331,10 +6353,10 @@
         <v>4</v>
       </c>
       <c r="Q25" t="s">
+        <v>426</v>
+      </c>
+      <c r="R25" t="s">
         <v>427</v>
-      </c>
-      <c r="R25" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="26" spans="2:18">
@@ -6381,10 +6403,10 @@
         <v>4</v>
       </c>
       <c r="Q26" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27" spans="2:18">
@@ -6407,10 +6429,10 @@
         <v>4</v>
       </c>
       <c r="Q27" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R27" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -6744,31 +6766,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
       <c r="P1" s="17"/>
     </row>
     <row r="2" spans="2:16" ht="15.75">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>410</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
       <c r="P2" s="17"/>
     </row>
     <row r="3" spans="2:16">
@@ -7432,16 +7454,16 @@
       <c r="P22" s="20"/>
     </row>
     <row r="23" spans="2:17" ht="15" thickBot="1">
-      <c r="M23" s="70" t="s">
+      <c r="M23" s="71" t="s">
         <v>409</v>
       </c>
-      <c r="N23" s="71"/>
-      <c r="O23" s="71"/>
-      <c r="P23" s="71"/>
-      <c r="Q23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+      <c r="Q23" s="73"/>
     </row>
     <row r="24" spans="2:17" ht="14.25" customHeight="1">
-      <c r="L24" s="67"/>
+      <c r="L24" s="68"/>
       <c r="M24" s="53" t="s">
         <v>339</v>
       </c>
@@ -7459,7 +7481,7 @@
       </c>
     </row>
     <row r="25" spans="2:17">
-      <c r="L25" s="67"/>
+      <c r="L25" s="68"/>
       <c r="M25" s="46" t="s">
         <v>411</v>
       </c>
@@ -7477,7 +7499,7 @@
       </c>
     </row>
     <row r="26" spans="2:17" ht="24">
-      <c r="L26" s="67"/>
+      <c r="L26" s="68"/>
       <c r="M26" s="48" t="s">
         <v>344</v>
       </c>
@@ -7495,7 +7517,7 @@
       </c>
     </row>
     <row r="27" spans="2:17" ht="24.75" thickBot="1">
-      <c r="L27" s="67"/>
+      <c r="L27" s="68"/>
       <c r="M27" s="50" t="s">
         <v>346</v>
       </c>

</xml_diff>